<commit_message>
Nuevas Mediciones 1 Rta Frec
Esta vez si esta la fase
</commit_message>
<xml_diff>
--- a/Ejercicio 1/mediciones .xlsx
+++ b/Ejercicio 1/mediciones .xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manueldieguez/Desktop/TP1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Desktop\TP01\Ejercicio 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6414B06-1988-496B-A95C-F9AD612DC2FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>frec</t>
   </si>
@@ -42,12 +51,174 @@
   </si>
   <si>
     <t>atenuacion</t>
+  </si>
+  <si>
+    <t>9.88</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>9.86</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>9.84</t>
+  </si>
+  <si>
+    <t>6.29</t>
+  </si>
+  <si>
+    <t>9.81</t>
+  </si>
+  <si>
+    <t>9.80</t>
+  </si>
+  <si>
+    <t>9.78</t>
+  </si>
+  <si>
+    <t>3.03</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>9.77</t>
+  </si>
+  <si>
+    <t>9.76</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>9.75</t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>9.74</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.166</t>
+  </si>
+  <si>
+    <t>0.124</t>
+  </si>
+  <si>
+    <t>9.73</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>0.048</t>
+  </si>
+  <si>
+    <t>3.92</t>
+  </si>
+  <si>
+    <t>4.98</t>
+  </si>
+  <si>
+    <t>0.038</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>0.096</t>
+  </si>
+  <si>
+    <t>0.292</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>9.72</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>9.71</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>9.67</t>
+  </si>
+  <si>
+    <t>9.59</t>
+  </si>
+  <si>
+    <t>4.59</t>
+  </si>
+  <si>
+    <t>5.79</t>
+  </si>
+  <si>
+    <t>9.53</t>
+  </si>
+  <si>
+    <t>9.48</t>
+  </si>
+  <si>
+    <t>6.65</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>9.45</t>
+  </si>
+  <si>
+    <t>7.63</t>
+  </si>
+  <si>
+    <t>9.42</t>
+  </si>
+  <si>
+    <t>7.93</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>9.39</t>
+  </si>
+  <si>
+    <t>8.16</t>
+  </si>
+  <si>
+    <t>9.38</t>
+  </si>
+  <si>
+    <t>8.32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -83,10 +254,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,6 +268,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -363,16 +538,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,7 +564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -403,8 +578,17 @@
         <f>-20+LOG10(C2/B2)</f>
         <v>-20.026635280028515</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <f xml:space="preserve"> 1000 + A2</f>
         <v>2000</v>
@@ -419,10 +603,19 @@
         <f t="shared" ref="D3:D33" si="0">-20+LOG10(C3/B3)</f>
         <v>-20.098600973542361</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="1" xml:space="preserve"> 1000 + A3</f>
+        <f t="shared" ref="A4:A11" si="1" xml:space="preserve"> 1000 + A3</f>
         <v>3000</v>
       </c>
       <c r="B4">
@@ -435,8 +628,17 @@
         <f t="shared" si="0"/>
         <v>-20.191533443137423</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>4000</v>
@@ -451,8 +653,17 @@
         <f t="shared" si="0"/>
         <v>-20.291583549581034</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>5000</v>
@@ -467,8 +678,17 @@
         <f t="shared" si="0"/>
         <v>-20.399997738416403</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>-67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>6000</v>
@@ -483,8 +703,17 @@
         <f t="shared" si="0"/>
         <v>-20.51383061630294</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>-72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>7000</v>
@@ -499,8 +728,17 @@
         <f t="shared" si="0"/>
         <v>-20.638809718822689</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>-78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>8000</v>
@@ -515,8 +753,17 @@
         <f t="shared" si="0"/>
         <v>-20.78601828083298</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <v>-82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9000</v>
@@ -531,8 +778,17 @@
         <f t="shared" si="0"/>
         <v>-20.975891136401792</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>-86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>10000</v>
@@ -547,8 +803,17 @@
         <f t="shared" si="0"/>
         <v>-21.267861632411325</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <f xml:space="preserve"> 10500</f>
         <v>10500</v>
@@ -563,8 +828,17 @@
         <f t="shared" si="0"/>
         <v>-21.498310553789601</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12">
+        <v>-95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10700</v>
       </c>
@@ -578,8 +852,17 @@
         <f t="shared" si="0"/>
         <v>-21.633009127687057</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13">
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10800</v>
       </c>
@@ -593,8 +876,17 @@
         <f t="shared" si="0"/>
         <v>-21.720159303405957</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10900</v>
       </c>
@@ -608,8 +900,17 @@
         <f t="shared" si="0"/>
         <v>-21.799340549453582</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>-102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>11000</v>
       </c>
@@ -623,8 +924,17 @@
         <f t="shared" si="0"/>
         <v>-21.933579309139844</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11100</v>
       </c>
@@ -638,8 +948,17 @@
         <f t="shared" si="0"/>
         <v>-22.129873954283813</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17">
+        <v>-116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11200</v>
       </c>
@@ -653,8 +972,17 @@
         <f t="shared" si="0"/>
         <v>-22.276001989962051</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18">
+        <v>-136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11300</v>
       </c>
@@ -668,8 +996,17 @@
         <f t="shared" si="0"/>
         <v>-22.196820743914426</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11400</v>
       </c>
@@ -683,8 +1020,17 @@
         <f t="shared" si="0"/>
         <v>-22.020729484858744</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11500</v>
       </c>
@@ -698,8 +1044,17 @@
         <f t="shared" si="0"/>
         <v>-21.895330446689705</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12000</v>
       </c>
@@ -713,8 +1068,17 @@
         <f t="shared" si="0"/>
         <v>-21.497390438017668</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13000</v>
       </c>
@@ -728,8 +1092,17 @@
         <f t="shared" si="0"/>
         <v>-21.167870928808991</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14000</v>
       </c>
@@ -743,8 +1116,17 @@
         <f t="shared" si="0"/>
         <v>-20.977954428829708</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20000</v>
       </c>
@@ -758,8 +1140,17 @@
         <f t="shared" si="0"/>
         <v>-20.548956964442258</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>30000</v>
       </c>
@@ -773,8 +1164,17 @@
         <f t="shared" si="0"/>
         <v>-20.312384746541102</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>40000</v>
       </c>
@@ -788,8 +1188,17 @@
         <f t="shared" si="0"/>
         <v>-20.212855540031835</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>50000</v>
       </c>
@@ -803,8 +1212,17 @@
         <f t="shared" si="0"/>
         <v>-20.146883987969893</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>60000</v>
       </c>
@@ -818,8 +1236,17 @@
         <f t="shared" si="0"/>
         <v>-20.110025872938085</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>70000</v>
       </c>
@@ -833,8 +1260,17 @@
         <f t="shared" si="0"/>
         <v>-20.085409514142597</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K30">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>80000</v>
       </c>
@@ -848,8 +1284,17 @@
         <f t="shared" si="0"/>
         <v>-20.067343804451117</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>53</v>
+      </c>
+      <c r="K31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>90000</v>
       </c>
@@ -863,8 +1308,17 @@
         <f t="shared" si="0"/>
         <v>-20.055344008688834</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>100000</v>
       </c>
@@ -877,6 +1331,15 @@
       <c r="D33">
         <f t="shared" si="0"/>
         <v>-20.045810579550643</v>
+      </c>
+      <c r="H33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregada superposicion de ltspice y medicion
</commit_message>
<xml_diff>
--- a/Ejercicio 1/mediciones .xlsx
+++ b/Ejercicio 1/mediciones .xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Desktop\TP01\Ejercicio 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Github\TP01\Ejercicio 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6414B06-1988-496B-A95C-F9AD612DC2FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E836E54-4488-4A44-AEB4-1DFF1FE1823B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>frec</t>
   </si>
@@ -51,168 +51,6 @@
   </si>
   <si>
     <t>atenuacion</t>
-  </si>
-  <si>
-    <t>9.88</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>9.86</t>
-  </si>
-  <si>
-    <t>7.8</t>
-  </si>
-  <si>
-    <t>9.84</t>
-  </si>
-  <si>
-    <t>6.29</t>
-  </si>
-  <si>
-    <t>9.81</t>
-  </si>
-  <si>
-    <t>9.80</t>
-  </si>
-  <si>
-    <t>9.78</t>
-  </si>
-  <si>
-    <t>3.03</t>
-  </si>
-  <si>
-    <t>2.26</t>
-  </si>
-  <si>
-    <t>9.77</t>
-  </si>
-  <si>
-    <t>9.76</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>9.75</t>
-  </si>
-  <si>
-    <t>1.05</t>
-  </si>
-  <si>
-    <t>9.74</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>0.34</t>
-  </si>
-  <si>
-    <t>0.26</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.166</t>
-  </si>
-  <si>
-    <t>0.124</t>
-  </si>
-  <si>
-    <t>9.73</t>
-  </si>
-  <si>
-    <t>0.084</t>
-  </si>
-  <si>
-    <t>0.048</t>
-  </si>
-  <si>
-    <t>3.92</t>
-  </si>
-  <si>
-    <t>4.98</t>
-  </si>
-  <si>
-    <t>0.038</t>
-  </si>
-  <si>
-    <t>0.06</t>
-  </si>
-  <si>
-    <t>0.096</t>
-  </si>
-  <si>
-    <t>0.292</t>
-  </si>
-  <si>
-    <t>0.65</t>
-  </si>
-  <si>
-    <t>9.72</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>9.71</t>
-  </si>
-  <si>
-    <t>2.7</t>
-  </si>
-  <si>
-    <t>9.67</t>
-  </si>
-  <si>
-    <t>9.59</t>
-  </si>
-  <si>
-    <t>4.59</t>
-  </si>
-  <si>
-    <t>5.79</t>
-  </si>
-  <si>
-    <t>9.53</t>
-  </si>
-  <si>
-    <t>9.48</t>
-  </si>
-  <si>
-    <t>6.65</t>
-  </si>
-  <si>
-    <t>7.2</t>
-  </si>
-  <si>
-    <t>9.45</t>
-  </si>
-  <si>
-    <t>7.63</t>
-  </si>
-  <si>
-    <t>9.42</t>
-  </si>
-  <si>
-    <t>7.93</t>
-  </si>
-  <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>9.39</t>
-  </si>
-  <si>
-    <t>8.16</t>
-  </si>
-  <si>
-    <t>9.38</t>
-  </si>
-  <si>
-    <t>8.32</t>
   </si>
 </sst>
 </file>
@@ -541,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -578,11 +416,15 @@
         <f>-20+LOG10(C2/B2)</f>
         <v>-20.026635280028515</v>
       </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
+      <c r="H2">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="I2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J2">
+        <f>20*LOG10(I2/H2)</f>
+        <v>-0.61938234484145793</v>
       </c>
       <c r="K2">
         <v>-21</v>
@@ -603,11 +445,15 @@
         <f t="shared" ref="D3:D33" si="0">-20+LOG10(C3/B3)</f>
         <v>-20.098600973542361</v>
       </c>
-      <c r="H3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
+      <c r="H3">
+        <v>9.86</v>
+      </c>
+      <c r="I3">
+        <v>7.8</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J33" si="1">20*LOG10(I3/H3)</f>
+        <v>-2.0356462450146156</v>
       </c>
       <c r="K3">
         <v>-37</v>
@@ -615,7 +461,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A11" si="1" xml:space="preserve"> 1000 + A3</f>
+        <f t="shared" ref="A4:A11" si="2" xml:space="preserve"> 1000 + A3</f>
         <v>3000</v>
       </c>
       <c r="B4">
@@ -628,11 +474,15 @@
         <f t="shared" si="0"/>
         <v>-20.191533443137423</v>
       </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
+      <c r="H4">
+        <v>9.84</v>
+      </c>
+      <c r="I4">
+        <v>6.29</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>-3.8868890597214509</v>
       </c>
       <c r="K4">
         <v>-50</v>
@@ -640,7 +490,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
       <c r="B5">
@@ -653,11 +503,15 @@
         <f t="shared" si="0"/>
         <v>-20.291583549581034</v>
       </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
+      <c r="H5">
+        <v>9.81</v>
+      </c>
+      <c r="I5">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>-5.8887932924046194</v>
       </c>
       <c r="K5">
         <v>-60</v>
@@ -665,7 +519,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5000</v>
       </c>
       <c r="B6">
@@ -678,11 +532,15 @@
         <f t="shared" si="0"/>
         <v>-20.399997738416403</v>
       </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>31</v>
+      <c r="H6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I6">
+        <v>3.92</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>-7.9588001734407534</v>
       </c>
       <c r="K6">
         <v>-67</v>
@@ -690,7 +548,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6000</v>
       </c>
       <c r="B7">
@@ -703,11 +561,15 @@
         <f t="shared" si="0"/>
         <v>-20.51383061630294</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>14</v>
+      <c r="H7">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>-10.177924525705928</v>
       </c>
       <c r="K7">
         <v>-72</v>
@@ -715,7 +577,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7000</v>
       </c>
       <c r="B8">
@@ -728,11 +590,15 @@
         <f t="shared" si="0"/>
         <v>-20.638809718822689</v>
       </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
+      <c r="H8">
+        <v>9.77</v>
+      </c>
+      <c r="I8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>-12.715722491427444</v>
       </c>
       <c r="K8">
         <v>-78</v>
@@ -740,7 +606,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8000</v>
       </c>
       <c r="B9">
@@ -753,11 +619,15 @@
         <f t="shared" si="0"/>
         <v>-20.78601828083298</v>
       </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
+      <c r="H9">
+        <v>9.76</v>
+      </c>
+      <c r="I9">
+        <v>2.6</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>-11.489529393917477</v>
       </c>
       <c r="K9">
         <v>-82</v>
@@ -765,7 +635,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9000</v>
       </c>
       <c r="B10">
@@ -778,11 +648,15 @@
         <f t="shared" si="0"/>
         <v>-20.975891136401792</v>
       </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
+      <c r="H10">
+        <v>9.75</v>
+      </c>
+      <c r="I10">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>-13.545015092855653</v>
       </c>
       <c r="K10">
         <v>-86</v>
@@ -790,7 +664,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
       <c r="B11">
@@ -803,11 +677,15 @@
         <f t="shared" si="0"/>
         <v>-21.267861632411325</v>
       </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
+      <c r="H11">
+        <v>9.74</v>
+      </c>
+      <c r="I11">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>-24.653682024122485</v>
       </c>
       <c r="K11">
         <v>-90</v>
@@ -828,11 +706,15 @@
         <f t="shared" si="0"/>
         <v>-21.498310553789601</v>
       </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>23</v>
+      <c r="H12">
+        <v>9.74</v>
+      </c>
+      <c r="I12">
+        <v>0.34</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>-29.141600796727207</v>
       </c>
       <c r="K12">
         <v>-95</v>
@@ -852,11 +734,15 @@
         <f t="shared" si="0"/>
         <v>-21.633009127687057</v>
       </c>
-      <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" t="s">
-        <v>24</v>
+      <c r="H13">
+        <v>9.74</v>
+      </c>
+      <c r="I13">
+        <v>0.26</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>-31.471712178155951</v>
       </c>
       <c r="K13">
         <v>-96</v>
@@ -876,11 +762,15 @@
         <f t="shared" si="0"/>
         <v>-21.720159303405957</v>
       </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>25</v>
+      <c r="H14">
+        <v>9.74</v>
+      </c>
+      <c r="I14">
+        <v>0.2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>-33.750579224292686</v>
       </c>
       <c r="K14">
         <v>-99</v>
@@ -900,11 +790,15 @@
         <f t="shared" si="0"/>
         <v>-21.799340549453582</v>
       </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
+      <c r="H15">
+        <v>9.74</v>
+      </c>
+      <c r="I15">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>-35.369017376771204</v>
       </c>
       <c r="K15">
         <v>-102</v>
@@ -924,11 +818,15 @@
         <f t="shared" si="0"/>
         <v>-21.933579309139844</v>
       </c>
-      <c r="H16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" t="s">
-        <v>27</v>
+      <c r="H16">
+        <v>9.73</v>
+      </c>
+      <c r="I16">
+        <v>0.124</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>-37.89382310212234</v>
       </c>
       <c r="K16">
         <v>-105</v>
@@ -948,11 +846,15 @@
         <f t="shared" si="0"/>
         <v>-22.129873954283813</v>
       </c>
-      <c r="H17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" t="s">
-        <v>29</v>
+      <c r="H17">
+        <v>9.73</v>
+      </c>
+      <c r="I17">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>-41.276671084129404</v>
       </c>
       <c r="K17">
         <v>-116</v>
@@ -972,11 +874,15 @@
         <f t="shared" si="0"/>
         <v>-22.276001989962051</v>
       </c>
-      <c r="H18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" t="s">
-        <v>30</v>
+      <c r="H18">
+        <v>9.73</v>
+      </c>
+      <c r="I18">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>-46.137432057855293</v>
       </c>
       <c r="K18">
         <v>-136</v>
@@ -996,11 +902,15 @@
         <f t="shared" si="0"/>
         <v>-22.196820743914426</v>
       </c>
-      <c r="H19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" t="s">
-        <v>33</v>
+      <c r="H19">
+        <v>9.73</v>
+      </c>
+      <c r="I19">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>-48.166584873030835</v>
       </c>
       <c r="K19">
         <v>165</v>
@@ -1020,11 +930,15 @@
         <f t="shared" si="0"/>
         <v>-22.020729484858744</v>
       </c>
-      <c r="H20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" t="s">
-        <v>34</v>
+      <c r="H20">
+        <v>9.73</v>
+      </c>
+      <c r="I20">
+        <v>0.06</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>-44.199231797694168</v>
       </c>
       <c r="K20">
         <v>123</v>
@@ -1044,11 +958,15 @@
         <f t="shared" si="0"/>
         <v>-21.895330446689705</v>
       </c>
-      <c r="H21" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" t="s">
-        <v>35</v>
+      <c r="H21">
+        <v>9.73</v>
+      </c>
+      <c r="I21">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>-40.116832144575667</v>
       </c>
       <c r="K21">
         <v>110</v>
@@ -1068,11 +986,15 @@
         <f t="shared" si="0"/>
         <v>-21.497390438017668</v>
       </c>
-      <c r="H22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" t="s">
-        <v>36</v>
+      <c r="H22">
+        <v>9.73</v>
+      </c>
+      <c r="I22">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>-30.454599776398673</v>
       </c>
       <c r="K22">
         <v>95</v>
@@ -1092,11 +1014,15 @@
         <f t="shared" si="0"/>
         <v>-21.167870928808991</v>
       </c>
-      <c r="H23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" t="s">
-        <v>37</v>
+      <c r="H23">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="I23">
+        <v>0.65</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>-23.495058165668379</v>
       </c>
       <c r="K23">
         <v>89</v>
@@ -1116,11 +1042,15 @@
         <f t="shared" si="0"/>
         <v>-20.977954428829708</v>
       </c>
-      <c r="H24" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" t="s">
-        <v>39</v>
+      <c r="H24">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>-19.744384598160099</v>
       </c>
       <c r="K24">
         <v>86</v>
@@ -1140,11 +1070,15 @@
         <f t="shared" si="0"/>
         <v>-20.548956964442258</v>
       </c>
-      <c r="H25" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" t="s">
-        <v>41</v>
+      <c r="H25">
+        <v>9.67</v>
+      </c>
+      <c r="I25">
+        <v>2.7</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>-11.081254198480286</v>
       </c>
       <c r="K25">
         <v>73</v>
@@ -1164,11 +1098,15 @@
         <f t="shared" si="0"/>
         <v>-20.312384746541102</v>
       </c>
-      <c r="H26" t="s">
-        <v>43</v>
-      </c>
-      <c r="I26" t="s">
-        <v>44</v>
+      <c r="H26">
+        <v>9.59</v>
+      </c>
+      <c r="I26">
+        <v>4.59</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>-6.400118432668048</v>
       </c>
       <c r="K26">
         <v>60</v>
@@ -1188,11 +1126,15 @@
         <f t="shared" si="0"/>
         <v>-20.212855540031835</v>
       </c>
-      <c r="H27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" t="s">
-        <v>45</v>
+      <c r="H27">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="I27">
+        <v>5.79</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>-4.3282867382178027</v>
       </c>
       <c r="K27">
         <v>52</v>
@@ -1212,11 +1154,15 @@
         <f t="shared" si="0"/>
         <v>-20.146883987969893</v>
       </c>
-      <c r="H28" t="s">
-        <v>47</v>
-      </c>
-      <c r="I28" t="s">
-        <v>48</v>
+      <c r="H28">
+        <v>9.48</v>
+      </c>
+      <c r="I28">
+        <v>6.65</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>-3.0797338406992325</v>
       </c>
       <c r="K28">
         <v>45</v>
@@ -1236,11 +1182,15 @@
         <f t="shared" si="0"/>
         <v>-20.110025872938085</v>
       </c>
-      <c r="H29" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" t="s">
-        <v>49</v>
+      <c r="H29">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="I29">
+        <v>7.2</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>-2.3619862415598889</v>
       </c>
       <c r="K29">
         <v>39</v>
@@ -1260,11 +1210,15 @@
         <f t="shared" si="0"/>
         <v>-20.085409514142597</v>
       </c>
-      <c r="H30" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" t="s">
-        <v>51</v>
+      <c r="H30">
+        <v>9.42</v>
+      </c>
+      <c r="I30">
+        <v>7.63</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>-1.8305272967599375</v>
       </c>
       <c r="K30">
         <v>34</v>
@@ -1284,11 +1238,15 @@
         <f t="shared" si="0"/>
         <v>-20.067343804451117</v>
       </c>
-      <c r="H31" t="s">
-        <v>54</v>
-      </c>
-      <c r="I31" t="s">
-        <v>53</v>
+      <c r="H31">
+        <v>9.4</v>
+      </c>
+      <c r="I31">
+        <v>7.93</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>-1.4770933256418981</v>
       </c>
       <c r="K31">
         <v>30</v>
@@ -1308,11 +1266,15 @@
         <f t="shared" si="0"/>
         <v>-20.055344008688834</v>
       </c>
-      <c r="H32" t="s">
-        <v>55</v>
-      </c>
-      <c r="I32" t="s">
-        <v>56</v>
+      <c r="H32">
+        <v>9.39</v>
+      </c>
+      <c r="I32">
+        <v>8.16</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>-1.2195086702449958</v>
       </c>
       <c r="K32">
         <v>28</v>
@@ -1332,11 +1294,15 @@
         <f t="shared" si="0"/>
         <v>-20.045810579550643</v>
       </c>
-      <c r="H33" t="s">
-        <v>57</v>
-      </c>
-      <c r="I33" t="s">
-        <v>58</v>
+      <c r="H33">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="I33">
+        <v>8.32</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>-1.0415902417668113</v>
       </c>
       <c r="K33">
         <v>25</v>

</xml_diff>

<commit_message>
Agregada imagen de rta al escalon
</commit_message>
<xml_diff>
--- a/Ejercicio 1/mediciones .xlsx
+++ b/Ejercicio 1/mediciones .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Github\TP01\Ejercicio 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E836E54-4488-4A44-AEB4-1DFF1FE1823B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3AFCFD-F35B-4DAF-BDCD-BD98BE90AFCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>frec</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>atenuacion</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>dB</t>
+  </si>
+  <si>
+    <t>Fase</t>
   </si>
 </sst>
 </file>
@@ -96,7 +105,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +389,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -401,6 +410,18 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>

<commit_message>
Ejercicio 1, me faltaba pushear
</commit_message>
<xml_diff>
--- a/Ejercicio 1/mediciones .xlsx
+++ b/Ejercicio 1/mediciones .xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Github\TP01\Ejercicio 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Documents\GitHub\TP01\Ejercicio 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3AFCFD-F35B-4DAF-BDCD-BD98BE90AFCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A986EA8-F4E5-48AE-B541-0B732C522C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -23,9 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>frec</t>
   </si>
@@ -60,6 +57,15 @@
   </si>
   <si>
     <t>Fase</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>cambiados</t>
+  </si>
+  <si>
+    <t>original</t>
   </si>
 </sst>
 </file>
@@ -386,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -451,7 +457,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <f xml:space="preserve"> 1000 + A2</f>
         <v>2000</v>
@@ -480,7 +486,7 @@
         <v>-37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A11" si="2" xml:space="preserve"> 1000 + A3</f>
         <v>3000</v>
@@ -509,7 +515,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4000</v>
@@ -538,7 +544,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5000</v>
@@ -567,7 +573,7 @@
         <v>-67</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6000</v>
@@ -596,7 +602,7 @@
         <v>-72</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7000</v>
@@ -615,17 +621,26 @@
         <v>9.77</v>
       </c>
       <c r="I8">
-        <v>2.2599999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>-12.715722491427444</v>
+        <v>-11.498424314959102</v>
       </c>
       <c r="K8">
         <v>-78</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8000</v>
@@ -644,17 +659,26 @@
         <v>9.76</v>
       </c>
       <c r="I9">
-        <v>2.6</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>-11.489529393917477</v>
+        <v>-12.706827570385819</v>
       </c>
       <c r="K9">
         <v>-82</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9">
+        <v>2.6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9000</v>
@@ -683,7 +707,7 @@
         <v>-86</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10000</v>
@@ -712,7 +736,7 @@
         <v>-90</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <f xml:space="preserve"> 10500</f>
         <v>10500</v>
@@ -741,7 +765,7 @@
         <v>-95</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10700</v>
       </c>
@@ -769,7 +793,7 @@
         <v>-96</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10800</v>
       </c>
@@ -797,7 +821,7 @@
         <v>-99</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10900</v>
       </c>
@@ -825,7 +849,7 @@
         <v>-102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>11000</v>
       </c>

</xml_diff>